<commit_message>
Se agregó la funcionalidad de añadir datos a ciertos archivos
</commit_message>
<xml_diff>
--- a/alumnos.xlsx
+++ b/alumnos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo\Desktop\Node Js Proyects\Semana 17\Laboratorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo\Desktop\Node Js Proyects\Semana 17\Repositorio del Lab\Laboratorio1C2Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C30E230-8A15-4607-8A8D-101563D8B460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47099FE-BEDD-482B-A83B-5005C9C99B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Nombres</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t xml:space="preserve">Gabriela </t>
+  </si>
+  <si>
+    <t>Natalia</t>
+  </si>
+  <si>
+    <t>Daniela</t>
   </si>
 </sst>
 </file>
@@ -363,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -403,6 +409,22 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>